<commit_message>
chore(EM): cleanups & update assets
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C395DE-7479-42C3-AB55-0710F977C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD440D61-3257-49E5-94DF-5A9204C5405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19230" yWindow="1860" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2625" yWindow="2340" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="213">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -475,12 +475,6 @@
     <t>プレイヤーへの好感度</t>
   </si>
   <si>
-    <t>服务昵称</t>
-  </si>
-  <si>
-    <t>サービスニックネーム</t>
-  </si>
-  <si>
     <t>編集プロンプト</t>
   </si>
   <si>
@@ -548,12 +542,6 @@
   </si>
   <si>
     <t>总请求数：</t>
-  </si>
-  <si>
-    <t>成功：</t>
-  </si>
-  <si>
-    <t>失败：</t>
   </si>
   <si>
     <t>请求/分钟：</t>
@@ -597,6 +585,104 @@
     <t>无法打开参数文件
 {0}
 {1}</t>
+  </si>
+  <si>
+    <t>服务昵称 (&lt;color=red&gt;更改后需要重新编辑参数&lt;/color&gt;)</t>
+  </si>
+  <si>
+    <t>サービスニックネーム (&lt;color=red&gt;変更後にパラメータを再編集する必要がある&lt;/color&gt;)</t>
+  </si>
+  <si>
+    <t>&lt;color=green&gt;成功：&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>&lt;color=red&gt;失败：&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>em_ui_switch_scheduling</t>
+  </si>
+  <si>
+    <t>switching scheduling mode {0} -&gt; {1}</t>
+  </si>
+  <si>
+    <t>em_ui_scene_scheduled</t>
+  </si>
+  <si>
+    <t>scene play scheduled, retries={0}</t>
+  </si>
+  <si>
+    <t>em_ui_scene_requesting</t>
+  </si>
+  <si>
+    <t>scene requesting</t>
+  </si>
+  <si>
+    <t>em_ui_scene_parse_error</t>
+  </si>
+  <si>
+    <t>scene failed to parse scripts
+{0}</t>
+  </si>
+  <si>
+    <t>em_ui_scene_complete</t>
+  </si>
+  <si>
+    <t>scene received
+{0}</t>
+  </si>
+  <si>
+    <t>em_ui_scene_timeout</t>
+  </si>
+  <si>
+    <t>scene request timeout after {0}s</t>
+  </si>
+  <si>
+    <t>em_ui_scene_failed</t>
+  </si>
+  <si>
+    <t>scene request failed: {0}
+{1}</t>
+  </si>
+  <si>
+    <t>em_ui_scene_retry_end</t>
+  </si>
+  <si>
+    <t>em_ui_tokens_tpr</t>
+  </si>
+  <si>
+    <t>トークン/リクエスト:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">切换调度模式 {0} -&gt; {1}  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">场景请求中  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">场景演出计划中，重试次数={0}  </t>
+  </si>
+  <si>
+    <t>场景脚本解析失败
+{0}</t>
+  </si>
+  <si>
+    <t>场景已接收
+{0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">场景请求失败：{0}  </t>
+  </si>
+  <si>
+    <t>场景请求超时，{0} 秒</t>
+  </si>
+  <si>
+    <t>scene stopping retries</t>
+  </si>
+  <si>
+    <t>中止重试</t>
+  </si>
+  <si>
+    <t>令牌/请求：</t>
   </si>
 </sst>
 </file>
@@ -961,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -1123,10 +1209,10 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="23.25">
@@ -1171,10 +1257,10 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="46.5">
@@ -1227,146 +1313,146 @@
     </row>
     <row r="22" spans="1:4" ht="23.25">
       <c r="A22" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="23.25">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23.25">
       <c r="A24" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="23.25">
       <c r="A25" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="23.25">
       <c r="A26" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="23.25">
       <c r="A27" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.25">
       <c r="A28" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25">
       <c r="A29" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="23.25">
       <c r="A30" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25">
       <c r="A31" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="23.25">
       <c r="A32" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="69.75">
       <c r="A33" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25">
@@ -1838,58 +1924,112 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="23.25">
-      <c r="A73" s="5"/>
+      <c r="A73" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="23.25">
-      <c r="A74" s="5"/>
+      <c r="A74" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="23.25">
-      <c r="A75" s="5"/>
+      <c r="A75" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4" ht="23.25">
-      <c r="A76" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="46.5">
+      <c r="A76" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-    </row>
-    <row r="77" spans="1:4" ht="23.25">
-      <c r="A77" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="46.5">
+      <c r="A77" s="5" t="s">
+        <v>194</v>
+      </c>
       <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="23.25">
-      <c r="A78" s="5"/>
+      <c r="A78" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-    </row>
-    <row r="79" spans="1:4" ht="23.25">
-      <c r="A79" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="46.5">
+      <c r="A79" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="23.25">
-      <c r="A80" s="5"/>
+      <c r="A80" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="C80" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="23.25">
-      <c r="A81" s="5"/>
+      <c r="A81" s="5" t="s">
+        <v>201</v>
+      </c>
       <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="23.25">
       <c r="A82" s="5"/>

</xml_diff>

<commit_message>
feat(EM): too much stuff
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD440D61-3257-49E5-94DF-5A9204C5405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B1AF46-E114-47C7-A576-04BE79B9F6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2340" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20175" yWindow="3255" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="225">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -587,12 +587,6 @@
 {1}</t>
   </si>
   <si>
-    <t>服务昵称 (&lt;color=red&gt;更改后需要重新编辑参数&lt;/color&gt;)</t>
-  </si>
-  <si>
-    <t>サービスニックネーム (&lt;color=red&gt;変更後にパラメータを再編集する必要がある&lt;/color&gt;)</t>
-  </si>
-  <si>
     <t>&lt;color=green&gt;成功：&lt;/color&gt;</t>
   </si>
   <si>
@@ -683,6 +677,48 @@
   </si>
   <si>
     <t>令牌/请求：</t>
+  </si>
+  <si>
+    <t>em_ui_config_reset</t>
+  </si>
+  <si>
+    <t>「Elin with AI」の設定が{0}にリセットされました</t>
+  </si>
+  <si>
+    <t>Elin with AI 增强对话配置已重置为 {0}</t>
+  </si>
+  <si>
+    <t>服务昵称 (&lt;i&gt;更改后需要重新编辑参数&lt;/i&gt;)</t>
+  </si>
+  <si>
+    <t>サービスニックネーム (&lt;i&gt;変更後にパラメータを再編集する必要がある&lt;/i&gt;)</t>
+  </si>
+  <si>
+    <t>em_ui_config_open</t>
+  </si>
+  <si>
+    <t>打开Mod配置</t>
+  </si>
+  <si>
+    <t>Mod設定を開く</t>
+  </si>
+  <si>
+    <t>Emmersive配置已更改</t>
+  </si>
+  <si>
+    <t>em_ui_config_changed</t>
+  </si>
+  <si>
+    <t>Emmersive configuration changed</t>
+  </si>
+  <si>
+    <t>em_character_data_statuses</t>
+  </si>
+  <si>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>ステータス</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -1115,7 +1151,7 @@
       <c r="C5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1127,7 +1163,7 @@
       <c r="C6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1139,7 +1175,7 @@
       <c r="C7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1151,7 +1187,7 @@
       <c r="C8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1163,7 +1199,7 @@
       <c r="C9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1175,7 +1211,7 @@
       <c r="C10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1187,7 +1223,7 @@
       <c r="C11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1199,7 +1235,7 @@
       <c r="C12" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1211,7 +1247,7 @@
       <c r="C13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1223,7 +1259,7 @@
       <c r="C14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1235,7 +1271,7 @@
       <c r="C15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1247,7 +1283,7 @@
       <c r="C16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1257,10 +1293,10 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>182</v>
+        <v>215</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="46.5">
@@ -1283,7 +1319,7 @@
       <c r="C19" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1295,7 +1331,7 @@
       <c r="C20" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1307,7 +1343,7 @@
       <c r="C21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1332,7 +1368,7 @@
         <v>151</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23.25">
@@ -1344,7 +1380,7 @@
         <v>153</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="23.25">
@@ -1925,135 +1961,225 @@
     </row>
     <row r="73" spans="1:4" ht="23.25">
       <c r="A73" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25">
       <c r="A74" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25">
       <c r="A75" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="46.5">
       <c r="A76" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="46.5">
       <c r="A77" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25">
       <c r="A78" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="46.5">
       <c r="A79" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="23.25">
       <c r="A80" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="23.25">
       <c r="A81" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D81" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="23.25">
+      <c r="A82" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="23.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="D82" s="5" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="23.25">
-      <c r="A83" s="5"/>
+      <c r="A83" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="23.25">
-      <c r="A84" s="5"/>
+      <c r="A84" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="85" spans="1:4" ht="23.25">
-      <c r="A85" s="5"/>
+      <c r="A85" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="23.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" ht="23.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="1:4" ht="23.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="1:4" ht="23.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" ht="23.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="1:4" ht="23.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="1:4" ht="23.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="1:4" ht="23.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="1:4" ht="23.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="1:4" ht="23.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="1:4" ht="23.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat(EM): concurrent requests & system prompt rewrite
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA461BB3-4349-4FF6-A92A-0046EDDC00B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4856CC9-FF40-40CC-99C0-58D3CE3522C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="3345" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13635" yWindow="3495" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="239">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -752,6 +752,15 @@
   </si>
   <si>
     <t>室内</t>
+  </si>
+  <si>
+    <t>em_nearby_characters_relationships</t>
+  </si>
+  <si>
+    <t>角色羁绊</t>
+  </si>
+  <si>
+    <t>キャラクターの絆</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -2209,10 +2218,16 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25">
-      <c r="A91" s="5"/>
+      <c r="A91" s="5" t="s">
+        <v>236</v>
+      </c>
       <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="23.25">
       <c r="A92" s="5"/>
@@ -2243,6 +2258,36 @@
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="1:4" ht="23.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="1:4" ht="23.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="1:4" ht="23.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="1:4" ht="23.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="1:4" ht="23.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat(EM): add whitelist & important only mode
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8B8AAB-218C-4E16-B821-C2A4EB38B749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD95B1D4-753D-482E-B8CE-5C6555E96F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="2115" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10965" yWindow="2460" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="306">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -936,6 +936,33 @@
   </si>
   <si>
     <t>AI サービスのステータス: {0}</t>
+  </si>
+  <si>
+    <t>em_ui_global_cooldown</t>
+  </si>
+  <si>
+    <t>Global Request Cooldown(s)</t>
+  </si>
+  <si>
+    <t>em_ui_tab_whitelist</t>
+  </si>
+  <si>
+    <t>ホワイトリスト</t>
+  </si>
+  <si>
+    <t>白名单</t>
+  </si>
+  <si>
+    <t>全局请求间隔(s)</t>
+  </si>
+  <si>
+    <t>em_ui_whitelist</t>
+  </si>
+  <si>
+    <t>AIサービスホワイトリストモード：{0}</t>
+  </si>
+  <si>
+    <t>AI服务白名单模式: {0}</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1328,7 @@
   <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -2659,22 +2686,40 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25">
-      <c r="A113" s="5"/>
+      <c r="A113" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
+      <c r="C113" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="23.25">
-      <c r="A114" s="5"/>
+      <c r="A114" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="C114" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="115" spans="1:4" ht="23.25">
-      <c r="A115" s="5"/>
+      <c r="A115" s="5" t="s">
+        <v>303</v>
+      </c>
       <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
+      <c r="C115" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="116" spans="1:4" ht="23.25">
       <c r="A116" s="5"/>

</xml_diff>

<commit_message>
feat(EM): add blacklist mode
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD95B1D4-753D-482E-B8CE-5C6555E96F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4242362F-AA46-41CC-B3F7-F92863D9E8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10965" yWindow="2460" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21780" yWindow="2220" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="312">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -963,6 +963,24 @@
   </si>
   <si>
     <t>AI服务白名单模式: {0}</t>
+  </si>
+  <si>
+    <t>em_ui_active_blacklist</t>
+  </si>
+  <si>
+    <t>em_ui_active_whitelist</t>
+  </si>
+  <si>
+    <t>活跃的黑名单角色</t>
+  </si>
+  <si>
+    <t>活跃的白名单角色</t>
+  </si>
+  <si>
+    <t>アクティブなブラックリスト</t>
+  </si>
+  <si>
+    <t>アクティブなホワイトリスト</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -2722,16 +2740,28 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="23.25">
-      <c r="A116" s="5"/>
+      <c r="A116" s="5" t="s">
+        <v>306</v>
+      </c>
       <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
+      <c r="C116" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="117" spans="1:4" ht="23.25">
-      <c r="A117" s="5"/>
+      <c r="A117" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
+      <c r="C117" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>309</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat(EM): dedicated popup feed
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE52A6F-95D6-4E1A-B6E4-861367584C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD94B33-B820-4FEE-AAFF-3A0D41C647F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21780" yWindow="2220" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="2565" windowWidth="35790" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="318">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -992,12 +992,21 @@
   <si>
     <t>&lt;color=blue&gt;API設定ガイド&lt;/color&gt;</t>
   </si>
+  <si>
+    <t>em_ui_use_pop</t>
+  </si>
+  <si>
+    <t>启用弹出气泡</t>
+  </si>
+  <si>
+    <t>ポップアップバブルの表示</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,6 +1049,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F1115"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1061,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1073,6 +1088,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -2786,10 +2802,16 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25">
-      <c r="A119" s="5"/>
+      <c r="A119" s="5" t="s">
+        <v>315</v>
+      </c>
       <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="C119" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="120" spans="1:4" ht="23.25">
       <c r="A120" s="5"/>

</xml_diff>

<commit_message>
chore(PT): use mono forwarded System.Memory
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD94B33-B820-4FEE-AAFF-3A0D41C647F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88590F41-F042-431F-86AB-45F597BD403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12555" yWindow="2565" windowWidth="35790" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="324">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1000,6 +1000,24 @@
   </si>
   <si>
     <t>ポップアップバブルの表示</t>
+  </si>
+  <si>
+    <t>em_ui_filter</t>
+  </si>
+  <si>
+    <t>em_ui_add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">追加 </t>
+  </si>
+  <si>
+    <t>添加</t>
+  </si>
+  <si>
+    <t>最近对话过滤</t>
+  </si>
+  <si>
+    <t>最近の会話フィルター</t>
   </si>
 </sst>
 </file>
@@ -2814,16 +2832,28 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="23.25">
-      <c r="A120" s="5"/>
+      <c r="A120" s="5" t="s">
+        <v>318</v>
+      </c>
       <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
+      <c r="C120" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="121" spans="1:4" ht="23.25">
-      <c r="A121" s="5"/>
+      <c r="A121" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
+      <c r="C121" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="122" spans="1:4" ht="23.25">
       <c r="A122" s="5"/>

</xml_diff>

<commit_message>
feat(EM): add recent action filter
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
+++ b/Emmersive/package/LangMod/CN/emmersive_localizations_cn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD94B33-B820-4FEE-AAFF-3A0D41C647F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88590F41-F042-431F-86AB-45F597BD403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12555" yWindow="2565" windowWidth="35790" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="324">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1000,6 +1000,24 @@
   </si>
   <si>
     <t>ポップアップバブルの表示</t>
+  </si>
+  <si>
+    <t>em_ui_filter</t>
+  </si>
+  <si>
+    <t>em_ui_add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">追加 </t>
+  </si>
+  <si>
+    <t>添加</t>
+  </si>
+  <si>
+    <t>最近对话过滤</t>
+  </si>
+  <si>
+    <t>最近の会話フィルター</t>
   </si>
 </sst>
 </file>
@@ -2814,16 +2832,28 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="23.25">
-      <c r="A120" s="5"/>
+      <c r="A120" s="5" t="s">
+        <v>318</v>
+      </c>
       <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
+      <c r="C120" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="121" spans="1:4" ht="23.25">
-      <c r="A121" s="5"/>
+      <c r="A121" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
+      <c r="C121" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="122" spans="1:4" ht="23.25">
       <c r="A122" s="5"/>

</xml_diff>